<commit_message>
added calc of max working hour per month with substraction of weekends and public holidays, gui for my castle started
</commit_message>
<xml_diff>
--- a/invoicer/data_result/result.xlsx
+++ b/invoicer/data_result/result.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -462,7 +462,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>01.04.2024</t>
+          <t>01.05.2024</t>
         </is>
       </c>
       <c r="B2" s="1" t="inlineStr">
@@ -507,7 +507,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t xml:space="preserve">tests
+          <t xml:space="preserve">test automation for admin part
 </t>
         </is>
       </c>
@@ -536,7 +536,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t xml:space="preserve">pi planning day1
+          <t xml:space="preserve">pi planning day 1
 </t>
         </is>
       </c>
@@ -565,7 +565,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t xml:space="preserve">pi planning day2
+          <t xml:space="preserve">pi planning day 2
 </t>
         </is>
       </c>
@@ -594,7 +594,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t xml:space="preserve">tests
+          <t xml:space="preserve">creating pipeline for regression tests
 </t>
         </is>
       </c>
@@ -602,7 +602,7 @@
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>06.04.2024</t>
+          <t>06.05.2024</t>
         </is>
       </c>
       <c r="B7" s="1" t="inlineStr">
@@ -626,7 +626,7 @@
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>07.04.2024</t>
+          <t>07.05.2024</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
@@ -671,7 +671,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t xml:space="preserve">after weekend
+          <t xml:space="preserve">test automations for panels refactor
 </t>
         </is>
       </c>
@@ -700,7 +700,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t xml:space="preserve">after Weekend 2
+          <t xml:space="preserve">tests for admin acquirer and messages
 </t>
         </is>
       </c>
@@ -729,7 +729,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t xml:space="preserve">test
+          <t xml:space="preserve">refactor for waits
 </t>
         </is>
       </c>
@@ -758,7 +758,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t xml:space="preserve">long ago
+          <t xml:space="preserve">test automation refactor for waits and unused methods
 </t>
         </is>
       </c>
@@ -787,7 +787,7 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t xml:space="preserve">Final test!!!
+          <t xml:space="preserve">retest of bug for incorrect transaction failed message
 </t>
         </is>
       </c>
@@ -795,7 +795,7 @@
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>13.04.2024</t>
+          <t>13.05.2024</t>
         </is>
       </c>
       <c r="B14" s="1" t="inlineStr">
@@ -819,7 +819,7 @@
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>14.04.2024</t>
+          <t>14.05.2024</t>
         </is>
       </c>
       <c r="B15" s="1" t="inlineStr">
@@ -864,7 +864,7 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t xml:space="preserve">test1
+          <t xml:space="preserve">tests refactor
 </t>
         </is>
       </c>
@@ -893,7 +893,7 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t xml:space="preserve">testing
+          <t xml:space="preserve">prod deploy sanity tests, tests automation
 </t>
         </is>
       </c>
@@ -922,7 +922,7 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t xml:space="preserve">test
+          <t xml:space="preserve">automations for portal tests
 </t>
         </is>
       </c>
@@ -951,7 +951,7 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t xml:space="preserve">testtest2
+          <t xml:space="preserve">refactor of automated tests
 </t>
         </is>
       </c>
@@ -980,7 +980,7 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t xml:space="preserve">tests
+          <t xml:space="preserve">tests smell code fixes, updating repo
 </t>
         </is>
       </c>
@@ -988,7 +988,7 @@
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>20.04.2024</t>
+          <t>20.05.2024</t>
         </is>
       </c>
       <c r="B21" s="1" t="inlineStr">
@@ -1012,7 +1012,7 @@
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>21.04.2024</t>
+          <t>21.05.2024</t>
         </is>
       </c>
       <c r="B22" s="1" t="inlineStr">
@@ -1057,7 +1057,7 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t xml:space="preserve">tests
+          <t xml:space="preserve">refactor tests for class methods
 </t>
         </is>
       </c>
@@ -1086,7 +1086,7 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t xml:space="preserve">tests
+          <t xml:space="preserve">test automation for transaction details
 </t>
         </is>
       </c>
@@ -1115,7 +1115,7 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t xml:space="preserve">tests
+          <t xml:space="preserve">transaction advance filters automated tests, pipeline clarification meeting
 </t>
         </is>
       </c>
@@ -1144,7 +1144,7 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t xml:space="preserve">tests
+          <t xml:space="preserve">reseeding db meeting, automation tests
 </t>
         </is>
       </c>
@@ -1173,7 +1173,7 @@
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t xml:space="preserve">tests
+          <t xml:space="preserve">investigation for pipeline bugs, automation tests
 </t>
         </is>
       </c>
@@ -1181,7 +1181,7 @@
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>27.04.2024</t>
+          <t>27.05.2024</t>
         </is>
       </c>
       <c r="B28" s="1" t="inlineStr">
@@ -1205,7 +1205,7 @@
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>28.04.2024</t>
+          <t>28.05.2024</t>
         </is>
       </c>
       <c r="B29" s="1" t="inlineStr">
@@ -1250,7 +1250,7 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t xml:space="preserve">test2
+          <t xml:space="preserve">terminal tests refactor
 </t>
         </is>
       </c>
@@ -1279,14 +1279,38 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t xml:space="preserve">tests
+          <t xml:space="preserve">admin tests refactor
 </t>
         </is>
       </c>
     </row>
     <row r="32">
-      <c r="D32">
-        <f>SUM(D1:D31)</f>
+      <c r="A32" s="1" t="inlineStr">
+        <is>
+          <t>31.05.2024</t>
+        </is>
+      </c>
+      <c r="B32" s="1" t="inlineStr">
+        <is>
+          <t>John Doe</t>
+        </is>
+      </c>
+      <c r="C32" s="1" t="inlineStr">
+        <is>
+          <t>TestClient</t>
+        </is>
+      </c>
+      <c r="D32" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E32" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F32" s="1" t="inlineStr"/>
+    </row>
+    <row r="33">
+      <c r="D33">
+        <f>SUM(D1:D32)</f>
         <v/>
       </c>
     </row>

</xml_diff>